<commit_message>
As on Updated 13th Feb
</commit_message>
<xml_diff>
--- a/POMFramework_Sarathi/DataFiles/RunDatabasewithVPN.xlsx
+++ b/POMFramework_Sarathi/DataFiles/RunDatabasewithVPN.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="99">
   <si>
     <t>Iteration</t>
   </si>
@@ -753,7 +753,7 @@
   <dimension ref="A1:E275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>